<commit_message>
Update to version 3.0
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BCpUC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\BCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF11D8B-6961-42E1-8033-23B326896378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="2835" yWindow="1230" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="1" r:id="rId2"/>
-    <sheet name="BCpUC" sheetId="3" r:id="rId3"/>
+    <sheet name="Battery Calculations" sheetId="1" r:id="rId2"/>
+    <sheet name="Balance of System Calculations" sheetId="5" r:id="rId3"/>
+    <sheet name="BCpUC" sheetId="3" r:id="rId4"/>
+    <sheet name="BBoSCpUC" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>$/kW</t>
   </si>
@@ -123,9 +136,6 @@
   </si>
   <si>
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
-  </si>
-  <si>
-    <t>We adjust 2010 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
   <si>
     <t>BCpUC Battery Cost per Unit Capacity</t>
@@ -183,15 +193,166 @@
   <si>
     <t>learning.</t>
   </si>
+  <si>
+    <t>BCpUC Battery Balance of System Cost per Unit Capacity</t>
+  </si>
+  <si>
+    <t>Unit: $/MW</t>
+  </si>
+  <si>
+    <t>Balance of System</t>
+  </si>
+  <si>
+    <t>Table 3. Detailed Cost Breakdown for a 60-MW U.S. Li-ion Standalone Storage System with Durations of 0.5–4 Hours</t>
+  </si>
+  <si>
+    <t>60-MW, 4-hour Duration, 240-MWh</t>
+  </si>
+  <si>
+    <t>60-MW, 2-hour Duration, 120-MWh</t>
+  </si>
+  <si>
+    <t>60-MW, 1-hour Duration, 60-MWh</t>
+  </si>
+  <si>
+    <t>60-MW, 0.5-hour Duration, 30-MWh</t>
+  </si>
+  <si>
+    <t>Li-ion battery</t>
+  </si>
+  <si>
+    <t>Battery central inverter</t>
+  </si>
+  <si>
+    <t>Structural BOS</t>
+  </si>
+  <si>
+    <t>Electrical BOS</t>
+  </si>
+  <si>
+    <t>EPC overhead</t>
+  </si>
+  <si>
+    <t>Sales tax</t>
+  </si>
+  <si>
+    <t>∑ EPC cost</t>
+  </si>
+  <si>
+    <t>Land acquisition</t>
+  </si>
+  <si>
+    <t>Permitting fee</t>
+  </si>
+  <si>
+    <t>Interconnection fee</t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t>Developer overhead</t>
+  </si>
+  <si>
+    <t>EPC/developer net profit</t>
+  </si>
+  <si>
+    <t>∑ Developer cost</t>
+  </si>
+  <si>
+    <t>Total Cost ($)</t>
+  </si>
+  <si>
+    <t>$/W</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Model Component</t>
+  </si>
+  <si>
+    <t>Installation labor &amp; equipment</t>
+  </si>
+  <si>
+    <t>Balance of System Costs</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy19osti/71714.pdf</t>
+  </si>
+  <si>
+    <t>Page 12, Table 3</t>
+  </si>
+  <si>
+    <t>National Renewable Energy Laboratory</t>
+  </si>
+  <si>
+    <t>2018 U.S. Utility-Scale Photovoltaics Plus-Energy Storage System Costs Benchmark</t>
+  </si>
+  <si>
+    <t>Only the battery cost is affected by endogenous learning.  The "Balance of System"</t>
+  </si>
+  <si>
+    <t>costs are read directly from this variable and are not modified via endogenous learning</t>
+  </si>
+  <si>
+    <t>inside the simulator.</t>
+  </si>
+  <si>
+    <t>We use the largest (4-hour duration) for our estimate.</t>
+  </si>
+  <si>
+    <t>Balance of System (excl. sales tax)</t>
+  </si>
+  <si>
+    <t>Sales tax on balance of system elements</t>
+  </si>
+  <si>
+    <t>The "balance of system" should include all costs the utility must pay to purchase and</t>
+  </si>
+  <si>
+    <t>install the battery system, apart from the batteries themselves (and apart from sales</t>
+  </si>
+  <si>
+    <t>tax on the batteries).  This includes the inverter, labor, etc.</t>
+  </si>
+  <si>
+    <t>Currency Adjustment</t>
+  </si>
+  <si>
+    <t>2010 to 2012 USD</t>
+  </si>
+  <si>
+    <t>We adjust currency using the following conversion factors:</t>
+  </si>
+  <si>
+    <t>2018 $/W</t>
+  </si>
+  <si>
+    <t>2018 $/MW</t>
+  </si>
+  <si>
+    <t>2018 to 2012 USD</t>
+  </si>
+  <si>
+    <t>2012 $/MW</t>
+  </si>
+  <si>
+    <t>For the U.S. model, we assume the balance of system costs remain constant throughout the model run.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0;#,##0"/>
+    <numFmt numFmtId="170" formatCode="###0;###0"/>
+    <numFmt numFmtId="171" formatCode="###0.00;###0.00"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +429,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +464,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -333,6 +521,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -354,7 +684,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -383,16 +713,115 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,7 +856,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -441,7 +869,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$B$11</c:f>
+              <c:f>'Battery Calculations'!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -474,7 +902,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Calculations!$A$16,Calculations!$A$18,Calculations!$A$20,Calculations!$A$22,Calculations!$A$24,Calculations!$A$26,Calculations!$A$28,Calculations!$A$30,Calculations!$A$32,Calculations!$A$34,Calculations!$A$36,Calculations!$A$38,Calculations!$A$40,Calculations!$A$42,Calculations!$A$44,Calculations!$A$46,Calculations!$A$48,Calculations!$A$50,Calculations!$A$52)</c:f>
+              <c:f>('Battery Calculations'!$A$16,'Battery Calculations'!$A$18,'Battery Calculations'!$A$20,'Battery Calculations'!$A$22,'Battery Calculations'!$A$24,'Battery Calculations'!$A$26,'Battery Calculations'!$A$28,'Battery Calculations'!$A$30,'Battery Calculations'!$A$32,'Battery Calculations'!$A$34,'Battery Calculations'!$A$36,'Battery Calculations'!$A$38,'Battery Calculations'!$A$40,'Battery Calculations'!$A$42,'Battery Calculations'!$A$44,'Battery Calculations'!$A$46,'Battery Calculations'!$A$48,'Battery Calculations'!$A$50,'Battery Calculations'!$A$52)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -540,7 +968,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Calculations!$B$16,Calculations!$B$18,Calculations!$B$20,Calculations!$B$22,Calculations!$B$24,Calculations!$B$26,Calculations!$B$28,Calculations!$B$30,Calculations!$B$32,Calculations!$B$34,Calculations!$B$36,Calculations!$B$38,Calculations!$B$40,Calculations!$B$42,Calculations!$B$44,Calculations!$B$46,Calculations!$B$48,Calculations!$B$50,Calculations!$B$52)</c:f>
+              <c:f>('Battery Calculations'!$B$16,'Battery Calculations'!$B$18,'Battery Calculations'!$B$20,'Battery Calculations'!$B$22,'Battery Calculations'!$B$24,'Battery Calculations'!$B$26,'Battery Calculations'!$B$28,'Battery Calculations'!$B$30,'Battery Calculations'!$B$32,'Battery Calculations'!$B$34,'Battery Calculations'!$B$36,'Battery Calculations'!$B$38,'Battery Calculations'!$B$40,'Battery Calculations'!$B$42,'Battery Calculations'!$B$44,'Battery Calculations'!$B$46,'Battery Calculations'!$B$48,'Battery Calculations'!$B$50,'Battery Calculations'!$B$52)</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -756,7 +1184,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -813,7 +1240,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1093,12 +1526,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1107,126 +1538,218 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="26" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="28" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15">
+    <row r="29" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="30" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+    </row>
+    <row r="39" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
         <v>1.0549999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="59">
+        <v>0.9143273584567535</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B22" r:id="rId3" xr:uid="{CA93FE29-A0A0-406A-B94C-DC5006AB819F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1256,22 +1779,22 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1481,7 +2004,7 @@
         <v>135.565</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1492,7 +2015,7 @@
         <v>133.44999999999999</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1702,7 +2225,7 @@
         <v>2010</v>
       </c>
       <c r="C60" s="14">
-        <f>A60*About!$A$23</f>
+        <f>A60*About!$A$41</f>
         <v>636.16499999999996</v>
       </c>
     </row>
@@ -1714,7 +2237,7 @@
         <v>2010</v>
       </c>
       <c r="C61" s="14">
-        <f>A61*About!$A$23</f>
+        <f>A61*About!$A$41</f>
         <v>821.84499999999991</v>
       </c>
     </row>
@@ -1726,7 +2249,7 @@
         <v>2010</v>
       </c>
       <c r="C62" s="14">
-        <f>A62*About!$A$23</f>
+        <f>A62*About!$A$41</f>
         <v>750.1049999999999</v>
       </c>
     </row>
@@ -1738,7 +2261,7 @@
         <v>2010</v>
       </c>
       <c r="C63" s="14">
-        <f>A63*About!$A$23</f>
+        <f>A63*About!$A$41</f>
         <v>745.88499999999999</v>
       </c>
     </row>
@@ -1750,7 +2273,7 @@
         <v>2010</v>
       </c>
       <c r="C64" s="14">
-        <f>A64*About!$A$23</f>
+        <f>A64*About!$A$41</f>
         <v>672.03499999999997</v>
       </c>
     </row>
@@ -1785,7 +2308,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,11 +2873,802 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC34B27C-0BFA-4D35-874E-EA84BA74EBE0}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" style="20" customWidth="1"/>
+    <col min="2" max="13" width="11.28515625" style="20" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="23">
+        <v>50160000</v>
+      </c>
+      <c r="C4" s="26">
+        <v>209</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0.84</v>
+      </c>
+      <c r="E4" s="27">
+        <v>25080000</v>
+      </c>
+      <c r="F4" s="26">
+        <v>209</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0.42</v>
+      </c>
+      <c r="H4" s="27">
+        <v>12540000</v>
+      </c>
+      <c r="I4" s="26">
+        <v>209</v>
+      </c>
+      <c r="J4" s="24">
+        <v>0.21</v>
+      </c>
+      <c r="K4" s="27">
+        <v>6270000</v>
+      </c>
+      <c r="L4" s="26">
+        <v>209</v>
+      </c>
+      <c r="M4" s="24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="C5" s="26">
+        <v>18</v>
+      </c>
+      <c r="D5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E5" s="27">
+        <v>4200000</v>
+      </c>
+      <c r="F5" s="26">
+        <v>35</v>
+      </c>
+      <c r="G5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H5" s="27">
+        <v>4200000</v>
+      </c>
+      <c r="I5" s="26">
+        <v>70</v>
+      </c>
+      <c r="J5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K5" s="27">
+        <v>4200000</v>
+      </c>
+      <c r="L5" s="26">
+        <v>140</v>
+      </c>
+      <c r="M5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="23">
+        <v>3121131</v>
+      </c>
+      <c r="C6" s="26">
+        <v>13</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1813452</v>
+      </c>
+      <c r="F6" s="26">
+        <v>15</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="H6" s="27">
+        <v>1159612</v>
+      </c>
+      <c r="I6" s="26">
+        <v>19</v>
+      </c>
+      <c r="J6" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="K6" s="27">
+        <v>832692</v>
+      </c>
+      <c r="L6" s="26">
+        <v>28</v>
+      </c>
+      <c r="M6" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="23">
+        <v>8602825</v>
+      </c>
+      <c r="C7" s="26">
+        <v>36</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E7" s="27">
+        <v>6119167</v>
+      </c>
+      <c r="F7" s="26">
+        <v>51</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="27">
+        <v>4877337</v>
+      </c>
+      <c r="I7" s="26">
+        <v>81</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0.08</v>
+      </c>
+      <c r="K7" s="27">
+        <v>4256423</v>
+      </c>
+      <c r="L7" s="26">
+        <v>142</v>
+      </c>
+      <c r="M7" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="23">
+        <v>5479149</v>
+      </c>
+      <c r="C8" s="26">
+        <v>23</v>
+      </c>
+      <c r="D8" s="24">
+        <v>0.09</v>
+      </c>
+      <c r="E8" s="27">
+        <v>4322275</v>
+      </c>
+      <c r="F8" s="26">
+        <v>36</v>
+      </c>
+      <c r="G8" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H8" s="27">
+        <v>3743838</v>
+      </c>
+      <c r="I8" s="26">
+        <v>62</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="K8" s="27">
+        <v>3454619</v>
+      </c>
+      <c r="L8" s="26">
+        <v>115</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="23">
+        <v>2775545</v>
+      </c>
+      <c r="C9" s="26">
+        <v>12</v>
+      </c>
+      <c r="D9" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="27">
+        <v>1948565</v>
+      </c>
+      <c r="F9" s="26">
+        <v>16</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1535075</v>
+      </c>
+      <c r="I9" s="26">
+        <v>26</v>
+      </c>
+      <c r="J9" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K9" s="27">
+        <v>1328330</v>
+      </c>
+      <c r="L9" s="26">
+        <v>44</v>
+      </c>
+      <c r="M9" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="23">
+        <v>5293460</v>
+      </c>
+      <c r="C10" s="26">
+        <v>22</v>
+      </c>
+      <c r="D10" s="24">
+        <v>0.09</v>
+      </c>
+      <c r="E10" s="27">
+        <v>3083292</v>
+      </c>
+      <c r="F10" s="26">
+        <v>26</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1978209</v>
+      </c>
+      <c r="I10" s="26">
+        <v>33</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K10" s="27">
+        <v>1425667</v>
+      </c>
+      <c r="L10" s="26">
+        <v>48</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="43">
+        <v>79632110</v>
+      </c>
+      <c r="C11" s="44">
+        <v>332</v>
+      </c>
+      <c r="D11" s="45">
+        <v>1.33</v>
+      </c>
+      <c r="E11" s="46">
+        <v>46566751</v>
+      </c>
+      <c r="F11" s="44">
+        <v>388</v>
+      </c>
+      <c r="G11" s="45">
+        <v>0.78</v>
+      </c>
+      <c r="H11" s="46">
+        <v>30034071</v>
+      </c>
+      <c r="I11" s="44">
+        <v>501</v>
+      </c>
+      <c r="J11" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="46">
+        <v>21767732</v>
+      </c>
+      <c r="L11" s="44">
+        <v>726</v>
+      </c>
+      <c r="M11" s="45">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="21">
+        <v>250000</v>
+      </c>
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>250000</v>
+      </c>
+      <c r="F12" s="22">
+        <v>2</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>250000</v>
+      </c>
+      <c r="I12" s="22">
+        <v>4</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0</v>
+      </c>
+      <c r="K12" s="28">
+        <v>250000</v>
+      </c>
+      <c r="L12" s="22">
+        <v>8</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="23">
+        <v>295289</v>
+      </c>
+      <c r="C13" s="26">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="27">
+        <v>295289</v>
+      </c>
+      <c r="F13" s="26">
+        <v>2</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <v>295289</v>
+      </c>
+      <c r="I13" s="26">
+        <v>5</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27">
+        <v>295289</v>
+      </c>
+      <c r="L13" s="26">
+        <v>10</v>
+      </c>
+      <c r="M13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="23">
+        <v>1802363</v>
+      </c>
+      <c r="C14" s="26">
+        <v>8</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1802363</v>
+      </c>
+      <c r="F14" s="26">
+        <v>15</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1802363</v>
+      </c>
+      <c r="I14" s="26">
+        <v>30</v>
+      </c>
+      <c r="J14" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K14" s="27">
+        <v>1802363</v>
+      </c>
+      <c r="L14" s="26">
+        <v>60</v>
+      </c>
+      <c r="M14" s="24">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="23">
+        <v>2477135</v>
+      </c>
+      <c r="C15" s="26">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1476303</v>
+      </c>
+      <c r="F15" s="26">
+        <v>12</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="H15" s="27">
+        <v>975887</v>
+      </c>
+      <c r="I15" s="26">
+        <v>16</v>
+      </c>
+      <c r="J15" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="K15" s="27">
+        <v>725679</v>
+      </c>
+      <c r="L15" s="26">
+        <v>24</v>
+      </c>
+      <c r="M15" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="23">
+        <v>2477135</v>
+      </c>
+      <c r="C16" s="26">
+        <v>10</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1476303</v>
+      </c>
+      <c r="F16" s="26">
+        <v>12</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="H16" s="27">
+        <v>975887</v>
+      </c>
+      <c r="I16" s="26">
+        <v>16</v>
+      </c>
+      <c r="J16" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="27">
+        <v>725679</v>
+      </c>
+      <c r="L16" s="26">
+        <v>24</v>
+      </c>
+      <c r="M16" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="23">
+        <v>4346702</v>
+      </c>
+      <c r="C17" s="26">
+        <v>18</v>
+      </c>
+      <c r="D17" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E17" s="27">
+        <v>2593350</v>
+      </c>
+      <c r="F17" s="26">
+        <v>22</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="H17" s="27">
+        <v>1716675</v>
+      </c>
+      <c r="I17" s="26">
+        <v>29</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K17" s="27">
+        <v>1278337</v>
+      </c>
+      <c r="L17" s="26">
+        <v>43</v>
+      </c>
+      <c r="M17" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="48">
+        <v>11648623</v>
+      </c>
+      <c r="C18" s="49">
+        <v>49</v>
+      </c>
+      <c r="D18" s="50">
+        <v>0.19</v>
+      </c>
+      <c r="E18" s="51">
+        <v>7893608</v>
+      </c>
+      <c r="F18" s="49">
+        <v>66</v>
+      </c>
+      <c r="G18" s="50">
+        <v>0.13</v>
+      </c>
+      <c r="H18" s="51">
+        <v>6016101</v>
+      </c>
+      <c r="I18" s="49">
+        <v>100</v>
+      </c>
+      <c r="J18" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="51">
+        <v>5077347</v>
+      </c>
+      <c r="L18" s="49">
+        <v>169</v>
+      </c>
+      <c r="M18" s="50">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="55">
+        <f>SUM(D5:D9,D12:D17)</f>
+        <v>0.57999999999999985</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="57">
+        <f>D10*SUM(D5:D7)/SUM(D4:D7)</f>
+        <v>2.1272727272727273E-2</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="55">
+        <f>SUM(D22:D23)</f>
+        <v>0.60127272727272707</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="60">
+        <f>D24*10^6</f>
+        <v>601272.72727272706</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="60">
+        <f>D25*About!A42</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF003399"/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2374,372 +3688,592 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>Calculations!A80</f>
-        <v>2014</v>
+        <f>'Battery Calculations'!A84</f>
+        <v>2018</v>
       </c>
       <c r="B2" s="9">
-        <f>Calculations!C80*1000</f>
-        <v>635681.28648150526</v>
+        <f>'Battery Calculations'!C84*1000</f>
+        <v>561998.2359458115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>Calculations!A81</f>
-        <v>2015</v>
+        <f>'Battery Calculations'!A85</f>
+        <v>2019</v>
       </c>
       <c r="B3" s="9">
-        <f>Calculations!C81*1000</f>
-        <v>615679.62000688352</v>
+        <f>'Battery Calculations'!C85*1000</f>
+        <v>545192.00172863714</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>Calculations!A82</f>
-        <v>2016</v>
+        <f>'Battery Calculations'!A86</f>
+        <v>2020</v>
       </c>
       <c r="B4" s="9">
-        <f>Calculations!C82*1000</f>
-        <v>596629.85829409957</v>
+        <f>'Battery Calculations'!C86*1000</f>
+        <v>528728.2359458115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>Calculations!A83</f>
-        <v>2017</v>
+        <f>'Battery Calculations'!A87</f>
+        <v>2021</v>
       </c>
       <c r="B5" s="9">
-        <f>Calculations!C83*1000</f>
-        <v>578532.00134338625</v>
+        <f>'Battery Calculations'!C87*1000</f>
+        <v>515659.62116147205</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>Calculations!A84</f>
-        <v>2018</v>
+        <f>'Battery Calculations'!A88</f>
+        <v>2022</v>
       </c>
       <c r="B6" s="9">
-        <f>Calculations!C84*1000</f>
-        <v>561998.2359458115</v>
+        <f>'Battery Calculations'!C88*1000</f>
+        <v>502568.2359458115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>Calculations!A85</f>
-        <v>2019</v>
+        <f>'Battery Calculations'!A89</f>
+        <v>2023</v>
       </c>
       <c r="B7" s="9">
-        <f>Calculations!C85*1000</f>
-        <v>545192.00172863714</v>
+        <f>'Battery Calculations'!C89*1000</f>
+        <v>489934.8596421238</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>Calculations!A86</f>
-        <v>2020</v>
+        <f>'Battery Calculations'!A90</f>
+        <v>2024</v>
       </c>
       <c r="B8" s="9">
-        <f>Calculations!C86*1000</f>
-        <v>528728.2359458115</v>
+        <f>'Battery Calculations'!C90*1000</f>
+        <v>478998.23594581155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>Calculations!A87</f>
-        <v>2021</v>
+        <f>'Battery Calculations'!A91</f>
+        <v>2025</v>
       </c>
       <c r="B9" s="9">
-        <f>Calculations!C87*1000</f>
-        <v>515659.62116147205</v>
+        <f>'Battery Calculations'!C91*1000</f>
+        <v>468017.71717082523</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>Calculations!A88</f>
-        <v>2022</v>
+        <f>'Battery Calculations'!A92</f>
+        <v>2026</v>
       </c>
       <c r="B10" s="9">
-        <f>Calculations!C88*1000</f>
-        <v>502568.2359458115</v>
+        <f>'Battery Calculations'!C92*1000</f>
+        <v>458538.2359458115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>Calculations!A89</f>
-        <v>2023</v>
+        <f>'Battery Calculations'!A93</f>
+        <v>2027</v>
       </c>
       <c r="B11" s="9">
-        <f>Calculations!C89*1000</f>
-        <v>489934.8596421238</v>
+        <f>'Battery Calculations'!C93*1000</f>
+        <v>449908.19374757633</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>Calculations!A90</f>
-        <v>2024</v>
+        <f>'Battery Calculations'!A94</f>
+        <v>2028</v>
       </c>
       <c r="B12" s="9">
-        <f>Calculations!C90*1000</f>
-        <v>478998.23594581155</v>
+        <f>'Battery Calculations'!C94*1000</f>
+        <v>442128.23594581155</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>Calculations!A91</f>
-        <v>2025</v>
+        <f>'Battery Calculations'!A95</f>
+        <v>2029</v>
       </c>
       <c r="B13" s="9">
-        <f>Calculations!C91*1000</f>
-        <v>468017.71717082523</v>
+        <f>'Battery Calculations'!C95*1000</f>
+        <v>435606.2893723771</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>Calculations!A92</f>
-        <v>2026</v>
+        <f>'Battery Calculations'!A96</f>
+        <v>2030</v>
       </c>
       <c r="B14" s="9">
-        <f>Calculations!C92*1000</f>
-        <v>458538.2359458115</v>
+        <f>'Battery Calculations'!C96*1000</f>
+        <v>429848.2359458115</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>Calculations!A93</f>
-        <v>2027</v>
+      <c r="A15" s="15">
+        <f>'Battery Calculations'!A97</f>
+        <v>2031</v>
       </c>
       <c r="B15" s="9">
-        <f>Calculations!C93*1000</f>
-        <v>449908.19374757633</v>
+        <f>'Battery Calculations'!C97*1000</f>
+        <v>427733.2359458115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>Calculations!A94</f>
-        <v>2028</v>
+      <c r="A16" s="15">
+        <f>'Battery Calculations'!A98</f>
+        <v>2032</v>
       </c>
       <c r="B16" s="9">
-        <f>Calculations!C94*1000</f>
-        <v>442128.23594581155</v>
+        <f>'Battery Calculations'!C98*1000</f>
+        <v>425618.2359458115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>Calculations!A95</f>
-        <v>2029</v>
+      <c r="A17" s="15">
+        <f>'Battery Calculations'!A99</f>
+        <v>2033</v>
       </c>
       <c r="B17" s="9">
-        <f>Calculations!C95*1000</f>
-        <v>435606.2893723771</v>
+        <f>'Battery Calculations'!C99*1000</f>
+        <v>424088.23594581144</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>Calculations!A96</f>
-        <v>2030</v>
+      <c r="A18" s="15">
+        <f>'Battery Calculations'!A100</f>
+        <v>2034</v>
       </c>
       <c r="B18" s="9">
-        <f>Calculations!C96*1000</f>
-        <v>429848.2359458115</v>
+        <f>'Battery Calculations'!C100*1000</f>
+        <v>422558.2359458115</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <f>Calculations!A97</f>
-        <v>2031</v>
+        <f>'Battery Calculations'!A101</f>
+        <v>2035</v>
       </c>
       <c r="B19" s="9">
-        <f>Calculations!C97*1000</f>
-        <v>427733.2359458115</v>
+        <f>'Battery Calculations'!C101*1000</f>
+        <v>421328.23594581144</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
-        <f>Calculations!A98</f>
-        <v>2032</v>
+        <f>'Battery Calculations'!A102</f>
+        <v>2036</v>
       </c>
       <c r="B20" s="9">
-        <f>Calculations!C98*1000</f>
-        <v>425618.2359458115</v>
+        <f>'Battery Calculations'!C102*1000</f>
+        <v>420098.2359458115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
-        <f>Calculations!A99</f>
-        <v>2033</v>
+        <f>'Battery Calculations'!A103</f>
+        <v>2037</v>
       </c>
       <c r="B21" s="9">
-        <f>Calculations!C99*1000</f>
-        <v>424088.23594581144</v>
+        <f>'Battery Calculations'!C103*1000</f>
+        <v>419023.2359458115</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
-        <f>Calculations!A100</f>
-        <v>2034</v>
+        <f>'Battery Calculations'!A104</f>
+        <v>2038</v>
       </c>
       <c r="B22" s="9">
-        <f>Calculations!C100*1000</f>
-        <v>422558.2359458115</v>
+        <f>'Battery Calculations'!C104*1000</f>
+        <v>417948.23594581144</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <f>Calculations!A101</f>
-        <v>2035</v>
+        <f>'Battery Calculations'!A105</f>
+        <v>2039</v>
       </c>
       <c r="B23" s="9">
-        <f>Calculations!C101*1000</f>
-        <v>421328.23594581144</v>
+        <f>'Battery Calculations'!C105*1000</f>
+        <v>416938.2359458115</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
-        <f>Calculations!A102</f>
-        <v>2036</v>
+        <f>'Battery Calculations'!A106</f>
+        <v>2040</v>
       </c>
       <c r="B24" s="9">
-        <f>Calculations!C102*1000</f>
-        <v>420098.2359458115</v>
+        <f>'Battery Calculations'!C106*1000</f>
+        <v>415928.2359458115</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
-        <f>Calculations!A103</f>
-        <v>2037</v>
+        <f>'Battery Calculations'!A107</f>
+        <v>2041</v>
       </c>
       <c r="B25" s="9">
-        <f>Calculations!C103*1000</f>
-        <v>419023.2359458115</v>
+        <f>'Battery Calculations'!C107*1000</f>
+        <v>414848.2359458115</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
-        <f>Calculations!A104</f>
-        <v>2038</v>
+        <f>'Battery Calculations'!A108</f>
+        <v>2042</v>
       </c>
       <c r="B26" s="9">
-        <f>Calculations!C104*1000</f>
-        <v>417948.23594581144</v>
+        <f>'Battery Calculations'!C108*1000</f>
+        <v>413768.2359458115</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
-        <f>Calculations!A105</f>
-        <v>2039</v>
+        <f>'Battery Calculations'!A109</f>
+        <v>2043</v>
       </c>
       <c r="B27" s="9">
-        <f>Calculations!C105*1000</f>
-        <v>416938.2359458115</v>
+        <f>'Battery Calculations'!C109*1000</f>
+        <v>412718.2359458115</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
-        <f>Calculations!A106</f>
-        <v>2040</v>
+        <f>'Battery Calculations'!A110</f>
+        <v>2044</v>
       </c>
       <c r="B28" s="9">
-        <f>Calculations!C106*1000</f>
-        <v>415928.2359458115</v>
+        <f>'Battery Calculations'!C110*1000</f>
+        <v>411668.2359458115</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
-        <f>Calculations!A107</f>
-        <v>2041</v>
+        <f>'Battery Calculations'!A111</f>
+        <v>2045</v>
       </c>
       <c r="B29" s="9">
-        <f>Calculations!C107*1000</f>
-        <v>414848.2359458115</v>
+        <f>'Battery Calculations'!C111*1000</f>
+        <v>410658.2359458115</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
-        <f>Calculations!A108</f>
-        <v>2042</v>
+        <f>'Battery Calculations'!A112</f>
+        <v>2046</v>
       </c>
       <c r="B30" s="9">
-        <f>Calculations!C108*1000</f>
-        <v>413768.2359458115</v>
+        <f>'Battery Calculations'!C112*1000</f>
+        <v>409648.2359458115</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
-        <f>Calculations!A109</f>
-        <v>2043</v>
+        <f>'Battery Calculations'!A113</f>
+        <v>2047</v>
       </c>
       <c r="B31" s="9">
-        <f>Calculations!C109*1000</f>
-        <v>412718.2359458115</v>
+        <f>'Battery Calculations'!C113*1000</f>
+        <v>408663.2359458115</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
-        <f>Calculations!A110</f>
-        <v>2044</v>
+        <f>'Battery Calculations'!A114</f>
+        <v>2048</v>
       </c>
       <c r="B32" s="9">
-        <f>Calculations!C110*1000</f>
-        <v>411668.2359458115</v>
+        <f>'Battery Calculations'!C114*1000</f>
+        <v>407678.2359458115</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
-        <f>Calculations!A111</f>
-        <v>2045</v>
+        <f>'Battery Calculations'!A115</f>
+        <v>2049</v>
       </c>
       <c r="B33" s="9">
-        <f>Calculations!C111*1000</f>
-        <v>410658.2359458115</v>
+        <f>'Battery Calculations'!C115*1000</f>
+        <v>406728.2359458115</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
-        <f>Calculations!A112</f>
+        <f>'Battery Calculations'!A116</f>
+        <v>2050</v>
+      </c>
+      <c r="B34" s="9">
+        <f>'Battery Calculations'!C116*1000</f>
+        <v>405778.2359458115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2600C7A-0160-47B2-B089-93F8CBD71882}">
+  <sheetPr>
+    <tabColor rgb="FF003399"/>
+  </sheetPr>
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1">
+        <v>2018</v>
+      </c>
+      <c r="C1">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="15">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="15">
+        <v>2022</v>
+      </c>
+      <c r="G1" s="15">
+        <v>2023</v>
+      </c>
+      <c r="H1" s="15">
+        <v>2024</v>
+      </c>
+      <c r="I1" s="15">
+        <v>2025</v>
+      </c>
+      <c r="J1" s="15">
+        <v>2026</v>
+      </c>
+      <c r="K1" s="15">
+        <v>2027</v>
+      </c>
+      <c r="L1" s="15">
+        <v>2028</v>
+      </c>
+      <c r="M1" s="15">
+        <v>2029</v>
+      </c>
+      <c r="N1" s="15">
+        <v>2030</v>
+      </c>
+      <c r="O1" s="15">
+        <v>2031</v>
+      </c>
+      <c r="P1" s="15">
+        <v>2032</v>
+      </c>
+      <c r="Q1" s="15">
+        <v>2033</v>
+      </c>
+      <c r="R1" s="15">
+        <v>2034</v>
+      </c>
+      <c r="S1" s="15">
+        <v>2035</v>
+      </c>
+      <c r="T1" s="15">
+        <v>2036</v>
+      </c>
+      <c r="U1" s="15">
+        <v>2037</v>
+      </c>
+      <c r="V1" s="15">
+        <v>2038</v>
+      </c>
+      <c r="W1" s="15">
+        <v>2039</v>
+      </c>
+      <c r="X1" s="15">
+        <v>2040</v>
+      </c>
+      <c r="Y1" s="15">
+        <v>2041</v>
+      </c>
+      <c r="Z1" s="15">
+        <v>2042</v>
+      </c>
+      <c r="AA1" s="15">
+        <v>2043</v>
+      </c>
+      <c r="AB1" s="15">
+        <v>2044</v>
+      </c>
+      <c r="AC1" s="15">
+        <v>2045</v>
+      </c>
+      <c r="AD1" s="15">
         <v>2046</v>
       </c>
-      <c r="B34" s="9">
-        <f>Calculations!C112*1000</f>
-        <v>409648.2359458115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
-        <f>Calculations!A113</f>
+      <c r="AE1" s="15">
         <v>2047</v>
       </c>
-      <c r="B35" s="9">
-        <f>Calculations!C113*1000</f>
-        <v>408663.2359458115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
-        <f>Calculations!A114</f>
+      <c r="AF1" s="15">
         <v>2048</v>
       </c>
-      <c r="B36" s="9">
-        <f>Calculations!C114*1000</f>
-        <v>407678.2359458115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <f>Calculations!A115</f>
+      <c r="AG1" s="15">
         <v>2049</v>
       </c>
-      <c r="B37" s="9">
-        <f>Calculations!C115*1000</f>
-        <v>406728.2359458115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
-        <f>Calculations!A116</f>
+      <c r="AH1" s="15">
         <v>2050</v>
       </c>
-      <c r="B38" s="9">
-        <f>Calculations!C116*1000</f>
-        <v>405778.2359458115</v>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9">
+        <f>'Balance of System Calculations'!D26</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="C2" s="9">
+        <f>$B2</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="D2" s="9">
+        <f t="shared" ref="D2:AH2" si="0">$B2</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="E2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="F2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="H2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="I2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="J2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="K2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="L2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="M2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="N2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="O2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="P2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="Q2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="R2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="S2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="T2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="U2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="V2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="W2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="X2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="Y2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="Z2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AA2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AB2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AC2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AD2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AE2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AF2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AG2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AH2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>